<commit_message>
finally settled user profile pic adding
</commit_message>
<xml_diff>
--- a/blueprints/db/routeSample.xlsx
+++ b/blueprints/db/routeSample.xlsx
@@ -4,16 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16640" windowHeight="10780" tabRatio="500" activeTab="1"/>
-    <workbookView xWindow="16600" yWindow="0" windowWidth="16880" windowHeight="9960" tabRatio="500" activeTab="2"/>
     <workbookView xWindow="16640" yWindow="9980" windowWidth="16880" windowHeight="9860" tabRatio="500" activeTab="3"/>
-    <workbookView xWindow="240" yWindow="10800" windowWidth="16420" windowHeight="9100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="transport-&gt;" sheetId="4" r:id="rId1"/>
-    <sheet name="route-&gt;" sheetId="1" r:id="rId2"/>
-    <sheet name="type-&gt;" sheetId="2" r:id="rId3"/>
-    <sheet name="time" sheetId="3" r:id="rId4"/>
+    <sheet name="busRoute-&gt;" sheetId="1" r:id="rId2"/>
+    <sheet name="busType-&gt;" sheetId="2" r:id="rId3"/>
+    <sheet name="busTime" sheetId="3" r:id="rId4"/>
+    <sheet name="busStations" sheetId="5" r:id="rId5"/>
+    <sheet name="currencyExchange" sheetId="6" r:id="rId6"/>
+    <sheet name="currencyCountry" sheetId="7" r:id="rId7"/>
+    <sheet name="busComments" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -25,14 +26,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="59">
   <si>
     <t>routeID</t>
   </si>
   <si>
-    <t>byUsername</t>
-  </si>
-  <si>
     <t>country</t>
   </si>
   <si>
@@ -42,12 +40,6 @@
     <t>toLocation</t>
   </si>
   <si>
-    <t>fromStationLocation</t>
-  </si>
-  <si>
-    <t>toStationLocation</t>
-  </si>
-  <si>
     <t>duration</t>
   </si>
   <si>
@@ -175,6 +167,42 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>train</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>gps</t>
+  </si>
+  <si>
+    <t>currentCurrency</t>
+  </si>
+  <si>
+    <t>toCurrency</t>
+  </si>
+  <si>
+    <t>exchangeRate</t>
+  </si>
+  <si>
+    <t>IRR</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>haha nice</t>
+  </si>
+  <si>
+    <t>9am is not correct</t>
+  </si>
+  <si>
+    <t>sounds legit</t>
+  </si>
+  <si>
+    <t>busRouteID</t>
   </si>
 </sst>
 </file>
@@ -215,12 +243,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -232,7 +266,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="51">
+  <cellStyleXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -284,14 +318,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="51">
+  <cellStyles count="67">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -317,6 +368,14 @@
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -342,6 +401,14 @@
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -671,20 +738,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
-    <sheetView workbookViewId="2"/>
-    <sheetView tabSelected="1" workbookViewId="3">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -692,7 +754,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -700,7 +762,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -708,7 +770,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -716,19 +778,24 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B5">
         <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -737,153 +804,117 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
-    <sheetView workbookViewId="2"/>
-    <sheetView workbookViewId="3"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="2" width="7.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="I1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2">
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1">
+        <v>40934</v>
+      </c>
+      <c r="F2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="1">
-        <v>40934</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="1">
+        <v>20</v>
+      </c>
+      <c r="E3" s="1">
         <v>40934</v>
       </c>
-      <c r="H3" s="2">
+      <c r="F3" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G4" s="1">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1">
         <v>40935</v>
       </c>
-      <c r="H4">
+      <c r="F4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="1">
+        <v>30</v>
+      </c>
+      <c r="E5" s="1">
         <v>40936</v>
       </c>
-      <c r="H5">
+      <c r="F5">
         <v>0</v>
       </c>
     </row>
@@ -893,9 +924,6 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -907,55 +935,50 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="I7" sqref="I7"/>
-    </sheetView>
-    <sheetView workbookViewId="2"/>
-    <sheetView workbookViewId="3"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="C1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2">
+      <c r="A2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="4">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G2">
         <v>9</v>
@@ -963,22 +986,22 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" t="s">
         <v>21</v>
       </c>
-      <c r="D3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E3" t="s">
-        <v>24</v>
-      </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G3">
         <v>22</v>
@@ -986,22 +1009,22 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G4">
         <v>3</v>
@@ -1009,22 +1032,22 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G5" s="3">
         <v>18.5</v>
@@ -1032,22 +1055,22 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G6" s="3">
         <v>8</v>
@@ -1055,22 +1078,22 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B7">
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G7">
         <v>18</v>
@@ -1078,22 +1101,22 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B8">
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G8">
         <v>9</v>
@@ -1101,21 +1124,18 @@
     </row>
     <row r="13" spans="1:9">
       <c r="I13" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="I14" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -1126,278 +1146,273 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
-    <sheetView tabSelected="1" workbookViewId="2">
-      <selection activeCell="I7" sqref="I7"/>
-    </sheetView>
-    <sheetView workbookViewId="3">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="C1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
         <v>38</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" t="s">
         <v>10</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B7">
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B8">
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B9">
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F9" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B10">
         <v>3</v>
       </c>
       <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
         <v>26</v>
       </c>
-      <c r="D10" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" t="s">
-        <v>29</v>
-      </c>
       <c r="F10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B11">
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E11" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F11" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B12">
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F12" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B13">
         <v>4</v>
       </c>
       <c r="C13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" t="s">
         <v>26</v>
       </c>
-      <c r="D13" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" t="s">
-        <v>29</v>
-      </c>
       <c r="F13" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1406,8 +1421,199 @@
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="22" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="17.5" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="30.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>